<commit_message>
BAU + other fixes
We introduced a BAU scenario as requested by Reviewer 1 of the Ecological Economics paper.
</commit_message>
<xml_diff>
--- a/Files for shocks/Full scale/hous_Full.xlsx
+++ b/Files for shocks/Full scale/hous_Full.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365.sharepoint.com/sites/DENG-SESAM/Documenti condivisi/PROJECTS/2023_H2020_FULFILL/Model/Files for shocks/Full scale/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/14a790445df90286/Documenti/GitHub/FULFILL_MARIO/Files for shocks/Full scale/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="224" documentId="13_ncr:1_{7C24BA5F-05B1-4FAD-A8B2-9B3659914889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94012AE6-0D04-49F9-A6A5-9A55783BA1F5}"/>
+  <xr:revisionPtr revIDLastSave="231" documentId="13_ncr:1_{7C24BA5F-05B1-4FAD-A8B2-9B3659914889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8E198EC-F5C4-4EDD-B49D-DC03FA52734A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hous_disaggregated" sheetId="3" r:id="rId1"/>
     <sheet name="hous" sheetId="2" r:id="rId2"/>
+    <sheet name="hous BAU" sheetId="4" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">hous_disaggregated!$A$1:$G$25</definedName>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="34">
   <si>
     <t>DK</t>
   </si>
@@ -654,7 +655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E159E65-8C96-AD41-8075-CB8C054C87CD}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
@@ -1248,7 +1249,7 @@
   <dimension ref="A1:AC18"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3320,16 +3321,2087 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9A5384-13EE-4D89-92F1-4C769AA81A1D}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:AC18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <f>IF([1]Foglio1!B$7=0,"IT",IF([1]Foglio1!B$7=1,"LV",IF([1]Foglio1!B$7=2,"DE",IF([1]Foglio1!B$7=3,"FR",IF([1]Foglio1!B$7=4,"DK")))))</f>
+        <v>DE</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <f>IF([1]Foglio1!C$7=0,"IT",IF([1]Foglio1!C$7=1,"LV",IF([1]Foglio1!C$7=2,"DE",IF([1]Foglio1!C$7=3,"FR",IF([1]Foglio1!C$7=4,"DK")))))</f>
+        <v>FR</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <f>IF([1]Foglio1!D$7=0,"IT",IF([1]Foglio1!D$7=1,"LV",IF([1]Foglio1!D$7=2,"DE",IF([1]Foglio1!D$7=3,"FR",IF([1]Foglio1!D$7=4,"DK")))))</f>
+        <v>LV</v>
+      </c>
+      <c r="F1" s="3" t="str">
+        <f>IF([1]Foglio1!E$7=0,"IT",IF([1]Foglio1!E$7=1,"LV",IF([1]Foglio1!E$7=2,"DE",IF([1]Foglio1!E$7=3,"FR",IF([1]Foglio1!E$7=4,"DK")))))</f>
+        <v>LV</v>
+      </c>
+      <c r="G1" s="3" t="str">
+        <f>IF([1]Foglio1!F$7=0,"IT",IF([1]Foglio1!F$7=1,"LV",IF([1]Foglio1!F$7=2,"DE",IF([1]Foglio1!F$7=3,"FR",IF([1]Foglio1!F$7=4,"DK")))))</f>
+        <v>DK</v>
+      </c>
+      <c r="H1" s="3" t="str">
+        <f>IF([1]Foglio1!G$7=0,"IT",IF([1]Foglio1!G$7=1,"LV",IF([1]Foglio1!G$7=2,"DE",IF([1]Foglio1!G$7=3,"FR",IF([1]Foglio1!G$7=4,"DK")))))</f>
+        <v>IT</v>
+      </c>
+      <c r="I1" s="3" t="str">
+        <f>IF([1]Foglio1!H$7=0,"IT",IF([1]Foglio1!H$7=1,"LV",IF([1]Foglio1!H$7=2,"DE",IF([1]Foglio1!H$7=3,"FR",IF([1]Foglio1!H$7=4,"DK")))))</f>
+        <v>DK</v>
+      </c>
+      <c r="J1" s="3" t="str">
+        <f>IF([1]Foglio1!I$7=0,"IT",IF([1]Foglio1!I$7=1,"LV",IF([1]Foglio1!I$7=2,"DE",IF([1]Foglio1!I$7=3,"FR",IF([1]Foglio1!I$7=4,"DK")))))</f>
+        <v>IT</v>
+      </c>
+      <c r="K1" s="3" t="str">
+        <f>IF([1]Foglio1!J$7=0,"IT",IF([1]Foglio1!J$7=1,"LV",IF([1]Foglio1!J$7=2,"DE",IF([1]Foglio1!J$7=3,"FR",IF([1]Foglio1!J$7=4,"DK")))))</f>
+        <v>FR</v>
+      </c>
+      <c r="L1" s="3" t="str">
+        <f>IF([1]Foglio1!K$7=0,"IT",IF([1]Foglio1!K$7=1,"LV",IF([1]Foglio1!K$7=2,"DE",IF([1]Foglio1!K$7=3,"FR",IF([1]Foglio1!K$7=4,"DK")))))</f>
+        <v>FR</v>
+      </c>
+      <c r="M1" s="3" t="str">
+        <f>IF([1]Foglio1!L$7=0,"IT",IF([1]Foglio1!L$7=1,"LV",IF([1]Foglio1!L$7=2,"DE",IF([1]Foglio1!L$7=3,"FR",IF([1]Foglio1!L$7=4,"DK")))))</f>
+        <v>DE</v>
+      </c>
+      <c r="N1" s="3" t="str">
+        <f>IF([1]Foglio1!M$7=0,"IT",IF([1]Foglio1!M$7=1,"LV",IF([1]Foglio1!M$7=2,"DE",IF([1]Foglio1!M$7=3,"FR",IF([1]Foglio1!M$7=4,"DK")))))</f>
+        <v>IT</v>
+      </c>
+      <c r="O1" s="3" t="str">
+        <f>IF([1]Foglio1!N$7=0,"IT",IF([1]Foglio1!N$7=1,"LV",IF([1]Foglio1!N$7=2,"DE",IF([1]Foglio1!N$7=3,"FR",IF([1]Foglio1!N$7=4,"DK")))))</f>
+        <v>IT</v>
+      </c>
+      <c r="P1" s="3" t="str">
+        <f>IF([1]Foglio1!O$7=0,"IT",IF([1]Foglio1!O$7=1,"LV",IF([1]Foglio1!O$7=2,"DE",IF([1]Foglio1!O$7=3,"FR",IF([1]Foglio1!O$7=4,"DK")))))</f>
+        <v>FR</v>
+      </c>
+      <c r="Q1" s="3" t="str">
+        <f>IF([1]Foglio1!P$7=0,"IT",IF([1]Foglio1!P$7=1,"LV",IF([1]Foglio1!P$7=2,"DE",IF([1]Foglio1!P$7=3,"FR",IF([1]Foglio1!P$7=4,"DK")))))</f>
+        <v>IT</v>
+      </c>
+      <c r="R1" s="3" t="str">
+        <f>IF([1]Foglio1!Q$7=0,"IT",IF([1]Foglio1!Q$7=1,"LV",IF([1]Foglio1!Q$7=2,"DE",IF([1]Foglio1!Q$7=3,"FR",IF([1]Foglio1!Q$7=4,"DK")))))</f>
+        <v>LV</v>
+      </c>
+      <c r="S1" s="3" t="str">
+        <f>IF([1]Foglio1!R$7=0,"IT",IF([1]Foglio1!R$7=1,"LV",IF([1]Foglio1!R$7=2,"DE",IF([1]Foglio1!R$7=3,"FR",IF([1]Foglio1!R$7=4,"DK")))))</f>
+        <v>IT</v>
+      </c>
+      <c r="T1" s="3" t="str">
+        <f>IF([1]Foglio1!S$7=0,"IT",IF([1]Foglio1!S$7=1,"LV",IF([1]Foglio1!S$7=2,"DE",IF([1]Foglio1!S$7=3,"FR",IF([1]Foglio1!S$7=4,"DK")))))</f>
+        <v>DK</v>
+      </c>
+      <c r="U1" s="3" t="str">
+        <f>IF([1]Foglio1!T$7=0,"IT",IF([1]Foglio1!T$7=1,"LV",IF([1]Foglio1!T$7=2,"DE",IF([1]Foglio1!T$7=3,"FR",IF([1]Foglio1!T$7=4,"DK")))))</f>
+        <v>DK</v>
+      </c>
+      <c r="V1" s="3" t="str">
+        <f>IF([1]Foglio1!U$7=0,"IT",IF([1]Foglio1!U$7=1,"LV",IF([1]Foglio1!U$7=2,"DE",IF([1]Foglio1!U$7=3,"FR",IF([1]Foglio1!U$7=4,"DK")))))</f>
+        <v>DK</v>
+      </c>
+      <c r="W1" s="3" t="str">
+        <f>IF([1]Foglio1!V$7=0,"IT",IF([1]Foglio1!V$7=1,"LV",IF([1]Foglio1!V$7=2,"DE",IF([1]Foglio1!V$7=3,"FR",IF([1]Foglio1!V$7=4,"DK")))))</f>
+        <v>LV</v>
+      </c>
+      <c r="X1" s="3" t="str">
+        <f>IF([1]Foglio1!W$7=0,"IT",IF([1]Foglio1!W$7=1,"LV",IF([1]Foglio1!W$7=2,"DE",IF([1]Foglio1!W$7=3,"FR",IF([1]Foglio1!W$7=4,"DK")))))</f>
+        <v>DE</v>
+      </c>
+      <c r="Y1" s="3" t="str">
+        <f>IF([1]Foglio1!X$7=0,"IT",IF([1]Foglio1!X$7=1,"LV",IF([1]Foglio1!X$7=2,"DE",IF([1]Foglio1!X$7=3,"FR",IF([1]Foglio1!X$7=4,"DK")))))</f>
+        <v>LV</v>
+      </c>
+      <c r="Z1" s="3" t="str">
+        <f>IF([1]Foglio1!Y$7=0,"IT",IF([1]Foglio1!Y$7=1,"LV",IF([1]Foglio1!Y$7=2,"DE",IF([1]Foglio1!Y$7=3,"FR",IF([1]Foglio1!Y$7=4,"DK")))))</f>
+        <v>LV</v>
+      </c>
+      <c r="AA1" s="3" t="str">
+        <f>IF([1]Foglio1!Z$7=0,"IT",IF([1]Foglio1!Z$7=1,"LV",IF([1]Foglio1!Z$7=2,"DE",IF([1]Foglio1!Z$7=3,"FR",IF([1]Foglio1!Z$7=4,"DK")))))</f>
+        <v>IT</v>
+      </c>
+      <c r="AB1" s="3" t="str">
+        <f>IF([1]Foglio1!AA$7=0,"IT",IF([1]Foglio1!AA$7=1,"LV",IF([1]Foglio1!AA$7=2,"DE",IF([1]Foglio1!AA$7=3,"FR",IF([1]Foglio1!AA$7=4,"DK")))))</f>
+        <v>FR</v>
+      </c>
+      <c r="AC1" s="3" t="str">
+        <f>IF([1]Foglio1!AB$7=0,"IT",IF([1]Foglio1!AB$7=1,"LV",IF([1]Foglio1!AB$7=2,"DE",IF([1]Foglio1!AB$7=3,"FR",IF([1]Foglio1!AB$7=4,"DK")))))</f>
+        <v>DE</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="6" cm="1">
+        <f t="array" ref="C3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!C$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!C$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.1490839694248394E-5</v>
+      </c>
+      <c r="D3" s="6" cm="1">
+        <f t="array" ref="D3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!D$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!D$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.1665409138296885E-5</v>
+      </c>
+      <c r="E3" s="6" cm="1">
+        <f t="array" ref="E3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!E$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!E$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.0535761330823824E-5</v>
+      </c>
+      <c r="F3" s="6" cm="1">
+        <f t="array" ref="F3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!F$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!F$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.0535761330823824E-5</v>
+      </c>
+      <c r="G3" s="6" cm="1">
+        <f t="array" ref="G3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!G$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!G$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.453688925801003E-5</v>
+      </c>
+      <c r="H3" s="6" cm="1">
+        <f t="array" ref="H3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!H$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!H$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.0479108784759777E-5</v>
+      </c>
+      <c r="I3" s="6" cm="1">
+        <f t="array" ref="I3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!I$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!I$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.453688925801003E-5</v>
+      </c>
+      <c r="J3" s="6" cm="1">
+        <f t="array" ref="J3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!J$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!J$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.0479108784759777E-5</v>
+      </c>
+      <c r="K3" s="6" cm="1">
+        <f t="array" ref="K3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!K$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!K$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.1665409138296885E-5</v>
+      </c>
+      <c r="L3" s="6" cm="1">
+        <f t="array" ref="L3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!L$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!L$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.1665409138296885E-5</v>
+      </c>
+      <c r="M3" s="6" cm="1">
+        <f t="array" ref="M3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!M$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!M$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.1490839694248394E-5</v>
+      </c>
+      <c r="N3" s="6" cm="1">
+        <f t="array" ref="N3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!N$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!N$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.0479108784759777E-5</v>
+      </c>
+      <c r="O3" s="6" cm="1">
+        <f t="array" ref="O3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!O$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!O$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.0479108784759777E-5</v>
+      </c>
+      <c r="P3" s="6" cm="1">
+        <f t="array" ref="P3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!P$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!P$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.1665409138296885E-5</v>
+      </c>
+      <c r="Q3" s="6" cm="1">
+        <f t="array" ref="Q3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!Q$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!Q$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.0479108784759777E-5</v>
+      </c>
+      <c r="R3" s="6" cm="1">
+        <f t="array" ref="R3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!R$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!R$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.0535761330823824E-5</v>
+      </c>
+      <c r="S3" s="6" cm="1">
+        <f t="array" ref="S3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!S$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!S$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.0479108784759777E-5</v>
+      </c>
+      <c r="T3" s="6" cm="1">
+        <f t="array" ref="T3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!T$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!T$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.453688925801003E-5</v>
+      </c>
+      <c r="U3" s="6" cm="1">
+        <f t="array" ref="U3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!U$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!U$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.453688925801003E-5</v>
+      </c>
+      <c r="V3" s="6" cm="1">
+        <f t="array" ref="V3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!V$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!V$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.453688925801003E-5</v>
+      </c>
+      <c r="W3" s="6" cm="1">
+        <f t="array" ref="W3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!W$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!W$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.0535761330823824E-5</v>
+      </c>
+      <c r="X3" s="6" cm="1">
+        <f t="array" ref="X3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!X$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!X$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.1490839694248394E-5</v>
+      </c>
+      <c r="Y3" s="6" cm="1">
+        <f t="array" ref="Y3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!Y$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!Y$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.0535761330823824E-5</v>
+      </c>
+      <c r="Z3" s="6" cm="1">
+        <f t="array" ref="Z3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!Z$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!Z$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.0535761330823824E-5</v>
+      </c>
+      <c r="AA3" s="6" cm="1">
+        <f t="array" ref="AA3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!AA$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!AA$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.0479108784759777E-5</v>
+      </c>
+      <c r="AB3" s="6" cm="1">
+        <f t="array" ref="AB3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!AB$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!AB$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.1665409138296885E-5</v>
+      </c>
+      <c r="AC3" s="6" cm="1">
+        <f t="array" ref="AC3">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!AC$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!AC$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A3),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.1490839694248394E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="5" cm="1">
+        <f t="array" ref="C4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!C$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>94.344620579376809</v>
+      </c>
+      <c r="D4" s="5" cm="1">
+        <f t="array" ref="D4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!D$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>75.348117501049643</v>
+      </c>
+      <c r="E4" s="5" cm="1">
+        <f t="array" ref="E4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!E$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>88.492977283820608</v>
+      </c>
+      <c r="F4" s="5" cm="1">
+        <f t="array" ref="F4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!F$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>88.492977283820608</v>
+      </c>
+      <c r="G4" s="5" cm="1">
+        <f t="array" ref="G4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!G$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>101.86366967947724</v>
+      </c>
+      <c r="H4" s="5" cm="1">
+        <f t="array" ref="H4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!H$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>53.673381592532138</v>
+      </c>
+      <c r="I4" s="5" cm="1">
+        <f t="array" ref="I4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!I$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>101.86366967947724</v>
+      </c>
+      <c r="J4" s="5" cm="1">
+        <f t="array" ref="J4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!J$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>53.673381592532138</v>
+      </c>
+      <c r="K4" s="5" cm="1">
+        <f t="array" ref="K4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!K$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>75.348117501049643</v>
+      </c>
+      <c r="L4" s="5" cm="1">
+        <f t="array" ref="L4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!L$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>75.348117501049643</v>
+      </c>
+      <c r="M4" s="5" cm="1">
+        <f t="array" ref="M4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!M$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>94.344620579376809</v>
+      </c>
+      <c r="N4" s="5" cm="1">
+        <f t="array" ref="N4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!N$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>53.673381592532138</v>
+      </c>
+      <c r="O4" s="5" cm="1">
+        <f t="array" ref="O4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!O$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>53.673381592532138</v>
+      </c>
+      <c r="P4" s="5" cm="1">
+        <f t="array" ref="P4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!P$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>75.348117501049643</v>
+      </c>
+      <c r="Q4" s="5" cm="1">
+        <f t="array" ref="Q4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!Q$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>53.673381592532138</v>
+      </c>
+      <c r="R4" s="5" cm="1">
+        <f t="array" ref="R4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!R$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>88.492977283820608</v>
+      </c>
+      <c r="S4" s="5" cm="1">
+        <f t="array" ref="S4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!S$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>53.673381592532138</v>
+      </c>
+      <c r="T4" s="5" cm="1">
+        <f t="array" ref="T4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!T$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>101.86366967947724</v>
+      </c>
+      <c r="U4" s="5" cm="1">
+        <f t="array" ref="U4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!U$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>101.86366967947724</v>
+      </c>
+      <c r="V4" s="5" cm="1">
+        <f t="array" ref="V4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!V$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>101.86366967947724</v>
+      </c>
+      <c r="W4" s="5" cm="1">
+        <f t="array" ref="W4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!W$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>88.492977283820608</v>
+      </c>
+      <c r="X4" s="5" cm="1">
+        <f t="array" ref="X4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!X$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>94.344620579376809</v>
+      </c>
+      <c r="Y4" s="5" cm="1">
+        <f t="array" ref="Y4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!Y$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>88.492977283820608</v>
+      </c>
+      <c r="Z4" s="5" cm="1">
+        <f t="array" ref="Z4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!Z$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>88.492977283820608</v>
+      </c>
+      <c r="AA4" s="5" cm="1">
+        <f t="array" ref="AA4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!AA$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>53.673381592532138</v>
+      </c>
+      <c r="AB4" s="5" cm="1">
+        <f t="array" ref="AB4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!AB$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>75.348117501049643</v>
+      </c>
+      <c r="AC4" s="5" cm="1">
+        <f t="array" ref="AC4">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A4)),hous_disaggregated!$C$1:$G$1='hous BAU'!AC$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B4)),0)</f>
+        <v>94.344620579376809</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="6" cm="1">
+        <f t="array" ref="C5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!C$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!C$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="D5" s="6" cm="1">
+        <f t="array" ref="D5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!D$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!D$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="E5" s="6" cm="1">
+        <f t="array" ref="E5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!E$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!E$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="F5" s="6" cm="1">
+        <f t="array" ref="F5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!F$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!F$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="G5" s="6" cm="1">
+        <f t="array" ref="G5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!G$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!G$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="H5" s="6" cm="1">
+        <f t="array" ref="H5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!H$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!H$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="I5" s="6" cm="1">
+        <f t="array" ref="I5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!I$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!I$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="J5" s="6" cm="1">
+        <f t="array" ref="J5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!J$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!J$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="K5" s="6" cm="1">
+        <f t="array" ref="K5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!K$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!K$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="L5" s="6" cm="1">
+        <f t="array" ref="L5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!L$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!L$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="M5" s="6" cm="1">
+        <f t="array" ref="M5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!M$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!M$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="N5" s="6" cm="1">
+        <f t="array" ref="N5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!N$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!N$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="O5" s="6" cm="1">
+        <f t="array" ref="O5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!O$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!O$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="P5" s="6" cm="1">
+        <f t="array" ref="P5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!P$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!P$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="Q5" s="6" cm="1">
+        <f t="array" ref="Q5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!Q$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!Q$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="R5" s="6" cm="1">
+        <f t="array" ref="R5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!R$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!R$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="S5" s="6" cm="1">
+        <f t="array" ref="S5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!S$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!S$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="T5" s="6" cm="1">
+        <f t="array" ref="T5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!T$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!T$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="U5" s="6" cm="1">
+        <f t="array" ref="U5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!U$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!U$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="V5" s="6" cm="1">
+        <f t="array" ref="V5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!V$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!V$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="W5" s="6" cm="1">
+        <f t="array" ref="W5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!W$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!W$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="X5" s="6" cm="1">
+        <f t="array" ref="X5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!X$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!X$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="Y5" s="6" cm="1">
+        <f t="array" ref="Y5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!Y$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!Y$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="Z5" s="6" cm="1">
+        <f t="array" ref="Z5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!Z$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!Z$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="AA5" s="6" cm="1">
+        <f t="array" ref="AA5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!AA$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!AA$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="AB5" s="6" cm="1">
+        <f t="array" ref="AB5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!AB$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!AB$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="AC5" s="6" cm="1">
+        <f t="array" ref="AC5">0.0000036*(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!AC$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Cooling need")+_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,hous_disaggregated!$C$1:$G$1='hous BAU'!AC$1),hous_disaggregated!$A$2:$A$25='hous BAU'!$A5),hous_disaggregated!$B$2:$B$4="Lighting need"))</f>
+        <v>8.2384134367494808E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="5" cm="1">
+        <f t="array" ref="C6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!C$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="D6" s="5" cm="1">
+        <f t="array" ref="D6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!D$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="E6" s="5" cm="1">
+        <f t="array" ref="E6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!E$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="F6" s="5" cm="1">
+        <f t="array" ref="F6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!F$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="G6" s="5" cm="1">
+        <f t="array" ref="G6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!G$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="H6" s="5" cm="1">
+        <f t="array" ref="H6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!H$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="I6" s="5" cm="1">
+        <f t="array" ref="I6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!I$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="J6" s="5" cm="1">
+        <f t="array" ref="J6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!J$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="K6" s="5" cm="1">
+        <f t="array" ref="K6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!K$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="L6" s="5" cm="1">
+        <f t="array" ref="L6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!L$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="M6" s="5" cm="1">
+        <f t="array" ref="M6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!M$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="N6" s="5" cm="1">
+        <f t="array" ref="N6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!N$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="O6" s="5" cm="1">
+        <f t="array" ref="O6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!O$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="P6" s="5" cm="1">
+        <f t="array" ref="P6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!P$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="Q6" s="5" cm="1">
+        <f t="array" ref="Q6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!Q$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="R6" s="5" cm="1">
+        <f t="array" ref="R6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!R$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="S6" s="5" cm="1">
+        <f t="array" ref="S6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!S$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="T6" s="5" cm="1">
+        <f t="array" ref="T6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!T$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="U6" s="5" cm="1">
+        <f t="array" ref="U6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!U$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="V6" s="5" cm="1">
+        <f t="array" ref="V6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!V$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="W6" s="5" cm="1">
+        <f t="array" ref="W6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!W$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="X6" s="5" cm="1">
+        <f t="array" ref="X6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!X$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="Y6" s="5" cm="1">
+        <f t="array" ref="Y6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!Y$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="Z6" s="5" cm="1">
+        <f t="array" ref="Z6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!Z$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="AA6" s="5" cm="1">
+        <f t="array" ref="AA6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!AA$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="AB6" s="5" cm="1">
+        <f t="array" ref="AB6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!AB$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="AC6" s="5" cm="1">
+        <f t="array" ref="AC6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(hous_disaggregated!$C$2:$G$25,(hous_disaggregated!$A$2:$A$25='hous BAU'!$A6)),hous_disaggregated!$C$1:$G$1='hous BAU'!AC$1),hous_disaggregated!$B$2:$B$4='hous BAU'!$B6)),0)</f>
+        <v>99.040930423849233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="6">
+        <f>C5</f>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" ref="D7:AC7" si="0">D5</f>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="0"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="0"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="K7" s="6">
+        <f t="shared" si="0"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="L7" s="6">
+        <f t="shared" si="0"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="M7" s="6">
+        <f t="shared" si="0"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="N7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="O7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="P7" s="6">
+        <f t="shared" si="0"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="Q7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="R7" s="6">
+        <f t="shared" si="0"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="S7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="T7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="U7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="V7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="W7" s="6">
+        <f t="shared" si="0"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="X7" s="6">
+        <f t="shared" si="0"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="Y7" s="6">
+        <f t="shared" si="0"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="Z7" s="6">
+        <f t="shared" si="0"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="AA7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="AB7" s="6">
+        <f t="shared" si="0"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="AC7" s="6">
+        <f t="shared" si="0"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" ref="C8:AC8" si="1">C6</f>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="1"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="1"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="1"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="1"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="1"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="1"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="1"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="K8" s="6">
+        <f t="shared" si="1"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" si="1"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="M8" s="6">
+        <f t="shared" si="1"/>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="N8" s="6">
+        <f t="shared" si="1"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="O8" s="6">
+        <f t="shared" si="1"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="P8" s="6">
+        <f t="shared" si="1"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="Q8" s="6">
+        <f t="shared" si="1"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="R8" s="6">
+        <f t="shared" si="1"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="S8" s="6">
+        <f t="shared" si="1"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="T8" s="6">
+        <f t="shared" si="1"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="U8" s="6">
+        <f t="shared" si="1"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="V8" s="6">
+        <f t="shared" si="1"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="W8" s="6">
+        <f t="shared" si="1"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="X8" s="6">
+        <f t="shared" si="1"/>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="Y8" s="6">
+        <f t="shared" si="1"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="Z8" s="6">
+        <f t="shared" si="1"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="AA8" s="6">
+        <f t="shared" si="1"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="AB8" s="6">
+        <f t="shared" si="1"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="AC8" s="6">
+        <f t="shared" si="1"/>
+        <v>99.040930423849233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>2030</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" ref="C9:AC9" si="2">C7</f>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" si="2"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="2"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="2"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="K9" s="6">
+        <f t="shared" si="2"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" si="2"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="M9" s="6">
+        <f t="shared" si="2"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="N9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="O9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="P9" s="6">
+        <f t="shared" si="2"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="Q9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="R9" s="6">
+        <f t="shared" si="2"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="S9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="T9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="U9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="V9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="W9" s="6">
+        <f t="shared" si="2"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="X9" s="6">
+        <f t="shared" si="2"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="Y9" s="6">
+        <f t="shared" si="2"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="Z9" s="6">
+        <f t="shared" si="2"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="AA9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="AB9" s="6">
+        <f t="shared" si="2"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="AC9" s="6">
+        <f t="shared" si="2"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>2030</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" ref="C10:AC10" si="3">C8</f>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="3"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="3"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="3"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="G10" s="6">
+        <f t="shared" si="3"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" si="3"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="3"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="3"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="K10" s="6">
+        <f t="shared" si="3"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="L10" s="6">
+        <f t="shared" si="3"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="M10" s="6">
+        <f t="shared" si="3"/>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="N10" s="6">
+        <f t="shared" si="3"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="O10" s="6">
+        <f t="shared" si="3"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="P10" s="6">
+        <f t="shared" si="3"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="Q10" s="6">
+        <f t="shared" si="3"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="R10" s="6">
+        <f t="shared" si="3"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="S10" s="6">
+        <f t="shared" si="3"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="T10" s="6">
+        <f t="shared" si="3"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="U10" s="6">
+        <f t="shared" si="3"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="V10" s="6">
+        <f t="shared" si="3"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="W10" s="6">
+        <f t="shared" si="3"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="X10" s="6">
+        <f t="shared" si="3"/>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="Y10" s="6">
+        <f t="shared" si="3"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="Z10" s="6">
+        <f t="shared" si="3"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="AA10" s="6">
+        <f t="shared" si="3"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="AB10" s="6">
+        <f t="shared" si="3"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="AC10" s="6">
+        <f t="shared" si="3"/>
+        <v>99.040930423849233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>2035</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" ref="C11:AC11" si="4">C9</f>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="D11" s="6">
+        <f t="shared" si="4"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="4"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="4"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="4"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="4"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="K11" s="6">
+        <f t="shared" si="4"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="L11" s="6">
+        <f t="shared" si="4"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="M11" s="6">
+        <f t="shared" si="4"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="N11" s="6">
+        <f t="shared" si="4"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="O11" s="6">
+        <f t="shared" si="4"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="P11" s="6">
+        <f t="shared" si="4"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="Q11" s="6">
+        <f t="shared" si="4"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="R11" s="6">
+        <f t="shared" si="4"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="S11" s="6">
+        <f t="shared" si="4"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="T11" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="U11" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="V11" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="W11" s="6">
+        <f t="shared" si="4"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="X11" s="6">
+        <f t="shared" si="4"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="Y11" s="6">
+        <f t="shared" si="4"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="Z11" s="6">
+        <f t="shared" si="4"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="AA11" s="6">
+        <f t="shared" si="4"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="AB11" s="6">
+        <f t="shared" si="4"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="AC11" s="6">
+        <f t="shared" si="4"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>2035</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" ref="C12:AC12" si="5">C10</f>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="D12" s="6">
+        <f t="shared" si="5"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="5"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="5"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="G12" s="6">
+        <f t="shared" si="5"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" si="5"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="5"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="5"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="5"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="5"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="M12" s="6">
+        <f t="shared" si="5"/>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="N12" s="6">
+        <f t="shared" si="5"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="O12" s="6">
+        <f t="shared" si="5"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="P12" s="6">
+        <f t="shared" si="5"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="Q12" s="6">
+        <f t="shared" si="5"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="R12" s="6">
+        <f t="shared" si="5"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="S12" s="6">
+        <f t="shared" si="5"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="T12" s="6">
+        <f t="shared" si="5"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="U12" s="6">
+        <f t="shared" si="5"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="V12" s="6">
+        <f t="shared" si="5"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="W12" s="6">
+        <f t="shared" si="5"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="X12" s="6">
+        <f t="shared" si="5"/>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="Y12" s="6">
+        <f t="shared" si="5"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="Z12" s="6">
+        <f t="shared" si="5"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="AA12" s="6">
+        <f t="shared" si="5"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="AB12" s="6">
+        <f t="shared" si="5"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="AC12" s="6">
+        <f t="shared" si="5"/>
+        <v>99.040930423849233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>2040</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" ref="C13:AC13" si="6">C11</f>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="D13" s="6">
+        <f t="shared" si="6"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="6"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" si="6"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="6"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="6"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="6"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="6"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="K13" s="6">
+        <f t="shared" si="6"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="L13" s="6">
+        <f t="shared" si="6"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="M13" s="6">
+        <f t="shared" si="6"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" si="6"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="O13" s="6">
+        <f t="shared" si="6"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="P13" s="6">
+        <f t="shared" si="6"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="Q13" s="6">
+        <f t="shared" si="6"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="R13" s="6">
+        <f t="shared" si="6"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="S13" s="6">
+        <f t="shared" si="6"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="T13" s="6">
+        <f t="shared" si="6"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="U13" s="6">
+        <f t="shared" si="6"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="V13" s="6">
+        <f t="shared" si="6"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="W13" s="6">
+        <f t="shared" si="6"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="X13" s="6">
+        <f t="shared" si="6"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="Y13" s="6">
+        <f t="shared" si="6"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="Z13" s="6">
+        <f t="shared" si="6"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="AA13" s="6">
+        <f t="shared" si="6"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="AB13" s="6">
+        <f t="shared" si="6"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="AC13" s="6">
+        <f t="shared" si="6"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>2040</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" ref="C14:AC14" si="7">C12</f>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" si="7"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="7"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="7"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="7"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="7"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="7"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="7"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="7"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="7"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="7"/>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="7"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="O14" s="6">
+        <f t="shared" si="7"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="P14" s="6">
+        <f t="shared" si="7"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="Q14" s="6">
+        <f t="shared" si="7"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="R14" s="6">
+        <f t="shared" si="7"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="S14" s="6">
+        <f t="shared" si="7"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="T14" s="6">
+        <f t="shared" si="7"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="U14" s="6">
+        <f t="shared" si="7"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="V14" s="6">
+        <f t="shared" si="7"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="W14" s="6">
+        <f t="shared" si="7"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="X14" s="6">
+        <f t="shared" si="7"/>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="Y14" s="6">
+        <f t="shared" si="7"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="Z14" s="6">
+        <f t="shared" si="7"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="AA14" s="6">
+        <f t="shared" si="7"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="AB14" s="6">
+        <f t="shared" si="7"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="AC14" s="6">
+        <f t="shared" si="7"/>
+        <v>99.040930423849233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>2045</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" ref="C15:AC15" si="8">C13</f>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="D15" s="6">
+        <f t="shared" si="8"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="8"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="8"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="8"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" si="8"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" si="8"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="J15" s="6">
+        <f t="shared" si="8"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="K15" s="6">
+        <f t="shared" si="8"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="L15" s="6">
+        <f t="shared" si="8"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="M15" s="6">
+        <f t="shared" si="8"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="N15" s="6">
+        <f t="shared" si="8"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="O15" s="6">
+        <f t="shared" si="8"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="P15" s="6">
+        <f t="shared" si="8"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="Q15" s="6">
+        <f t="shared" si="8"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="R15" s="6">
+        <f t="shared" si="8"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="S15" s="6">
+        <f t="shared" si="8"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="T15" s="6">
+        <f t="shared" si="8"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="U15" s="6">
+        <f t="shared" si="8"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="V15" s="6">
+        <f t="shared" si="8"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="W15" s="6">
+        <f t="shared" si="8"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="X15" s="6">
+        <f t="shared" si="8"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="Y15" s="6">
+        <f t="shared" si="8"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="Z15" s="6">
+        <f t="shared" si="8"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="AA15" s="6">
+        <f t="shared" si="8"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="AB15" s="6">
+        <f t="shared" si="8"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="AC15" s="6">
+        <f t="shared" si="8"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>2045</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" ref="C16:AC16" si="9">C14</f>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="D16" s="6">
+        <f t="shared" si="9"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" si="9"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="9"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="G16" s="6">
+        <f t="shared" si="9"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="H16" s="6">
+        <f t="shared" si="9"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="I16" s="6">
+        <f t="shared" si="9"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="J16" s="6">
+        <f t="shared" si="9"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="K16" s="6">
+        <f t="shared" si="9"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="L16" s="6">
+        <f t="shared" si="9"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="M16" s="6">
+        <f t="shared" si="9"/>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="N16" s="6">
+        <f t="shared" si="9"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="O16" s="6">
+        <f t="shared" si="9"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="P16" s="6">
+        <f t="shared" si="9"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="Q16" s="6">
+        <f t="shared" si="9"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="R16" s="6">
+        <f t="shared" si="9"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="S16" s="6">
+        <f t="shared" si="9"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="T16" s="6">
+        <f t="shared" si="9"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="U16" s="6">
+        <f t="shared" si="9"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="V16" s="6">
+        <f t="shared" si="9"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="W16" s="6">
+        <f t="shared" si="9"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="X16" s="6">
+        <f t="shared" si="9"/>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="Y16" s="6">
+        <f t="shared" si="9"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="Z16" s="6">
+        <f t="shared" si="9"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="AA16" s="6">
+        <f t="shared" si="9"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="AB16" s="6">
+        <f t="shared" si="9"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="AC16" s="6">
+        <f t="shared" si="9"/>
+        <v>99.040930423849233</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>2050</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" ref="C17:AC17" si="10">C15</f>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="D17" s="6">
+        <f t="shared" si="10"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="10"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="10"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="G17" s="6">
+        <f t="shared" si="10"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" si="10"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="I17" s="6">
+        <f t="shared" si="10"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="J17" s="6">
+        <f t="shared" si="10"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="K17" s="6">
+        <f t="shared" si="10"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="L17" s="6">
+        <f t="shared" si="10"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="M17" s="6">
+        <f t="shared" si="10"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="N17" s="6">
+        <f t="shared" si="10"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="O17" s="6">
+        <f t="shared" si="10"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="P17" s="6">
+        <f t="shared" si="10"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="Q17" s="6">
+        <f t="shared" si="10"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="R17" s="6">
+        <f t="shared" si="10"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="S17" s="6">
+        <f t="shared" si="10"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="T17" s="6">
+        <f t="shared" si="10"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="U17" s="6">
+        <f t="shared" si="10"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="V17" s="6">
+        <f t="shared" si="10"/>
+        <v>1.1348710792682708E-5</v>
+      </c>
+      <c r="W17" s="6">
+        <f t="shared" si="10"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="X17" s="6">
+        <f t="shared" si="10"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+      <c r="Y17" s="6">
+        <f t="shared" si="10"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="Z17" s="6">
+        <f t="shared" si="10"/>
+        <v>7.1038860500999108E-6</v>
+      </c>
+      <c r="AA17" s="6">
+        <f t="shared" si="10"/>
+        <v>1.2033969835785323E-5</v>
+      </c>
+      <c r="AB17" s="6">
+        <f t="shared" si="10"/>
+        <v>9.3236310549552314E-6</v>
+      </c>
+      <c r="AC17" s="6">
+        <f t="shared" si="10"/>
+        <v>8.2384134367494808E-6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>2050</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" ref="C18:AC18" si="11">C16</f>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="D18" s="6">
+        <f t="shared" si="11"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="11"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="11"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="11"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="11"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="11"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="11"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="11"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="11"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="M18" s="6">
+        <f t="shared" si="11"/>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" si="11"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="O18" s="6">
+        <f t="shared" si="11"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="P18" s="6">
+        <f t="shared" si="11"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="Q18" s="6">
+        <f t="shared" si="11"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="R18" s="6">
+        <f t="shared" si="11"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="S18" s="6">
+        <f t="shared" si="11"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="T18" s="6">
+        <f t="shared" si="11"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="U18" s="6">
+        <f t="shared" si="11"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="V18" s="6">
+        <f t="shared" si="11"/>
+        <v>99.79077322260099</v>
+      </c>
+      <c r="W18" s="6">
+        <f t="shared" si="11"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="X18" s="6">
+        <f t="shared" si="11"/>
+        <v>99.040930423849233</v>
+      </c>
+      <c r="Y18" s="6">
+        <f t="shared" si="11"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="Z18" s="6">
+        <f t="shared" si="11"/>
+        <v>84.967559229876272</v>
+      </c>
+      <c r="AA18" s="6">
+        <f t="shared" si="11"/>
+        <v>55.932722606408952</v>
+      </c>
+      <c r="AB18" s="6">
+        <f t="shared" si="11"/>
+        <v>71.017994446851063</v>
+      </c>
+      <c r="AC18" s="6">
+        <f t="shared" si="11"/>
+        <v>99.040930423849233</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100241E96938535DD4B921FCDFB54345D30" ma:contentTypeVersion="18" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="a5d5c10fb5d76e91b5d3863d63e8b979">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e" xmlns:ns3="e67e9a88-35e1-4b39-8da9-a609eb308282" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7cec042378b2404c094b5ca61f00f7c" ns2:_="" ns3:_="">
     <xsd:import namespace="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e"/>
@@ -3584,15 +5656,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F8E1EBC-79AB-4818-9339-12553028CEF9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DF80A0E-81E0-4835-95F6-C8CB89BB29EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3609,4 +5682,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F8E1EBC-79AB-4818-9339-12553028CEF9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>